<commit_message>
team name revised. Total health FC Lab.
</commit_message>
<xml_diff>
--- a/01_Docs/03_StartingOrder/60th_TGNC_StartingOrder.xlsx
+++ b/01_Docs/03_StartingOrder/60th_TGNC_StartingOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jpngym.sharepoint.com/sites/TRA885/Shared Documents/03_全日本選手権/2023/01_Docs/03_StartingOrder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="650" documentId="8_{694C7A62-5ED9-964C-8CFD-A299403CF838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F19E3A-5118-8745-AAB6-4A458B72D0F4}"/>
+  <xr:revisionPtr revIDLastSave="651" documentId="8_{694C7A62-5ED9-964C-8CFD-A299403CF838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E55E9045-F610-C648-A31C-9BC9B28DD86C}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="620" windowWidth="34160" windowHeight="28040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44780" yWindow="620" windowWidth="23880" windowHeight="28040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="使用しない Revise" sheetId="10" r:id="rId1"/>
@@ -1182,10 +1182,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>トータルヘルスからだ調律ラボ/フリーエアースポーツクラブ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>静岡トランポリンクラブ/城南静岡高等学校</t>
     <rPh sb="12" eb="20">
       <t>ジョウナン</t>
@@ -1824,6 +1820,9 @@
   <si>
     <t>T3</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>トータルヘルスFCラボ/フリーエアースポーツクラブ</t>
   </si>
 </sst>
 </file>
@@ -2608,7 +2607,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2620,10 +2631,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2635,10 +2646,19 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2650,22 +2670,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2675,15 +2698,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2701,21 +2715,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -2725,7 +2724,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="15">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2813,16 +2812,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7418,10 +7407,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="60"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="23"/>
@@ -7472,7 +7461,7 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -7490,8 +7479,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23">
-      <c r="A1" s="93" t="s">
-        <v>517</v>
+      <c r="A1" s="59" t="s">
+        <v>516</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -7531,14 +7520,14 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="63" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>222</v>
@@ -7552,7 +7541,7 @@
       <c r="J5" s="52"/>
     </row>
     <row r="6" spans="1:10" ht="16" customHeight="1">
-      <c r="A6" s="60"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -7571,7 +7560,7 @@
       <c r="J6" s="52"/>
     </row>
     <row r="7" spans="1:10" ht="16" customHeight="1">
-      <c r="A7" s="60"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -7590,7 +7579,7 @@
       <c r="J7" s="52"/>
     </row>
     <row r="8" spans="1:10" ht="16" customHeight="1">
-      <c r="A8" s="60"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -7607,7 +7596,7 @@
       <c r="J8" s="52"/>
     </row>
     <row r="9" spans="1:10" ht="16" customHeight="1">
-      <c r="A9" s="60"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -7624,7 +7613,7 @@
       <c r="J9" s="52"/>
     </row>
     <row r="10" spans="1:10" ht="16" customHeight="1">
-      <c r="A10" s="60"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -7641,7 +7630,7 @@
       <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1">
-      <c r="A11" s="60"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -7660,7 +7649,7 @@
       <c r="J11" s="52"/>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
-      <c r="A12" s="60"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -7677,7 +7666,7 @@
       <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:10" ht="16" customHeight="1">
-      <c r="A13" s="60"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -7694,7 +7683,7 @@
       <c r="J13" s="52"/>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A14" s="61"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="8">
         <v>10</v>
       </c>
@@ -7711,7 +7700,7 @@
       <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:10" ht="17" customHeight="1">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="63" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6">
@@ -7730,24 +7719,24 @@
       <c r="J15" s="52"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
-      <c r="A16" s="60"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="7">
         <v>2</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="F16" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>369</v>
-      </c>
       <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1">
-      <c r="A17" s="60"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="7">
         <v>3</v>
       </c>
@@ -7764,7 +7753,7 @@
       <c r="J17" s="52"/>
     </row>
     <row r="18" spans="1:10" ht="16" customHeight="1">
-      <c r="A18" s="60"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="7">
         <v>4</v>
       </c>
@@ -7781,7 +7770,7 @@
       <c r="J18" s="52"/>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
-      <c r="A19" s="60"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="7">
         <v>5</v>
       </c>
@@ -7798,7 +7787,7 @@
       <c r="J19" s="52"/>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1">
-      <c r="A20" s="60"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="7">
         <v>6</v>
       </c>
@@ -7817,7 +7806,7 @@
       <c r="J20" s="52"/>
     </row>
     <row r="21" spans="1:10" ht="16" customHeight="1">
-      <c r="A21" s="60"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="7">
         <v>7</v>
       </c>
@@ -7836,7 +7825,7 @@
       <c r="J21" s="52"/>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1">
-      <c r="A22" s="60"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="7">
         <v>8</v>
       </c>
@@ -7853,7 +7842,7 @@
       <c r="J22" s="52"/>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
-      <c r="A23" s="60"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="7">
         <v>9</v>
       </c>
@@ -7870,7 +7859,7 @@
       <c r="J23" s="52"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
-      <c r="A24" s="60"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="7">
         <v>10</v>
       </c>
@@ -7887,7 +7876,7 @@
       <c r="J24" s="52"/>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A25" s="61"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="8">
         <v>11</v>
       </c>
@@ -7906,7 +7895,7 @@
       <c r="J25" s="52"/>
     </row>
     <row r="26" spans="1:10" ht="17" customHeight="1">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="63" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="6">
@@ -7927,12 +7916,12 @@
       <c r="J26" s="52"/>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1">
-      <c r="A27" s="60"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="7">
         <v>2</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>220</v>
@@ -7946,7 +7935,7 @@
       <c r="J27" s="52"/>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1">
-      <c r="A28" s="60"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="7">
         <v>3</v>
       </c>
@@ -7963,7 +7952,7 @@
       <c r="J28" s="52"/>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1">
-      <c r="A29" s="60"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="7">
         <v>4</v>
       </c>
@@ -7982,7 +7971,7 @@
       <c r="J29" s="52"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1">
-      <c r="A30" s="60"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="7">
         <v>5</v>
       </c>
@@ -7999,7 +7988,7 @@
       <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1">
-      <c r="A31" s="60"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="7">
         <v>6</v>
       </c>
@@ -8016,7 +8005,7 @@
       <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1">
-      <c r="A32" s="60"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="7">
         <v>7</v>
       </c>
@@ -8033,7 +8022,7 @@
       <c r="J32" s="52"/>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1">
-      <c r="A33" s="60"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="7">
         <v>8</v>
       </c>
@@ -8050,7 +8039,7 @@
       <c r="J33" s="52"/>
     </row>
     <row r="34" spans="1:10" ht="16" customHeight="1">
-      <c r="A34" s="60"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="7">
         <v>9</v>
       </c>
@@ -8069,7 +8058,7 @@
       <c r="J34" s="52"/>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1">
-      <c r="A35" s="60"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="7">
         <v>10</v>
       </c>
@@ -8086,7 +8075,7 @@
       <c r="J35" s="52"/>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A36" s="61"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -8103,7 +8092,7 @@
       <c r="J36" s="52"/>
     </row>
     <row r="37" spans="1:10" ht="17" customHeight="1">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="63" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="6">
@@ -8124,7 +8113,7 @@
       <c r="J37" s="52"/>
     </row>
     <row r="38" spans="1:10" ht="16" customHeight="1">
-      <c r="A38" s="60"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="7">
         <v>2</v>
       </c>
@@ -8143,7 +8132,7 @@
       <c r="J38" s="52"/>
     </row>
     <row r="39" spans="1:10" ht="16" customHeight="1">
-      <c r="A39" s="60"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="7">
         <v>3</v>
       </c>
@@ -8160,13 +8149,13 @@
       <c r="J39" s="52"/>
     </row>
     <row r="40" spans="1:10" ht="16" customHeight="1">
-      <c r="A40" s="60"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="7">
         <v>4</v>
       </c>
       <c r="C40" s="39"/>
       <c r="D40" s="24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>277</v>
@@ -8177,7 +8166,7 @@
       <c r="J40" s="52"/>
     </row>
     <row r="41" spans="1:10" ht="16" customHeight="1">
-      <c r="A41" s="60"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="7">
         <v>5</v>
       </c>
@@ -8194,7 +8183,7 @@
       <c r="J41" s="52"/>
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1">
-      <c r="A42" s="60"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="7">
         <v>6</v>
       </c>
@@ -8213,7 +8202,7 @@
       <c r="J42" s="52"/>
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1">
-      <c r="A43" s="60"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="7">
         <v>7</v>
       </c>
@@ -8230,7 +8219,7 @@
       <c r="J43" s="52"/>
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1">
-      <c r="A44" s="60"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="7">
         <v>8</v>
       </c>
@@ -8249,7 +8238,7 @@
       <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10" ht="16" customHeight="1">
-      <c r="A45" s="60"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="7">
         <v>9</v>
       </c>
@@ -8268,7 +8257,7 @@
       <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1">
-      <c r="A46" s="60"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="7">
         <v>10</v>
       </c>
@@ -8285,7 +8274,7 @@
       <c r="J46" s="52"/>
     </row>
     <row r="47" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A47" s="61"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="8">
         <v>11</v>
       </c>
@@ -8302,7 +8291,7 @@
       <c r="J47" s="52"/>
     </row>
     <row r="48" spans="1:10" ht="17" customHeight="1">
-      <c r="A48" s="59" t="s">
+      <c r="A48" s="63" t="s">
         <v>75</v>
       </c>
       <c r="B48" s="6">
@@ -8323,7 +8312,7 @@
       <c r="J48" s="52"/>
     </row>
     <row r="49" spans="1:10" ht="16" customHeight="1">
-      <c r="A49" s="60"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="7">
         <v>2</v>
       </c>
@@ -8340,7 +8329,7 @@
       <c r="J49" s="52"/>
     </row>
     <row r="50" spans="1:10" ht="16" customHeight="1">
-      <c r="A50" s="60"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="7">
         <v>3</v>
       </c>
@@ -8357,7 +8346,7 @@
       <c r="J50" s="52"/>
     </row>
     <row r="51" spans="1:10" ht="16" customHeight="1">
-      <c r="A51" s="60"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="7">
         <v>4</v>
       </c>
@@ -8376,7 +8365,7 @@
       <c r="J51" s="52"/>
     </row>
     <row r="52" spans="1:10" ht="16" customHeight="1">
-      <c r="A52" s="60"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="7">
         <v>5</v>
       </c>
@@ -8395,7 +8384,7 @@
       <c r="J52" s="52"/>
     </row>
     <row r="53" spans="1:10" ht="16" customHeight="1">
-      <c r="A53" s="60"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="7">
         <v>6</v>
       </c>
@@ -8412,7 +8401,7 @@
       <c r="J53" s="52"/>
     </row>
     <row r="54" spans="1:10" ht="16" customHeight="1">
-      <c r="A54" s="60"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="7">
         <v>7</v>
       </c>
@@ -8429,12 +8418,12 @@
       <c r="J54" s="52"/>
     </row>
     <row r="55" spans="1:10" ht="16" customHeight="1">
-      <c r="A55" s="60"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="7">
         <v>8</v>
       </c>
       <c r="C55" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>88</v>
@@ -8448,7 +8437,7 @@
       <c r="J55" s="52"/>
     </row>
     <row r="56" spans="1:10" ht="16" customHeight="1">
-      <c r="A56" s="60"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="7">
         <v>9</v>
       </c>
@@ -8467,7 +8456,7 @@
       <c r="J56" s="52"/>
     </row>
     <row r="57" spans="1:10" ht="16" customHeight="1">
-      <c r="A57" s="60"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="7">
         <v>10</v>
       </c>
@@ -8475,7 +8464,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E57" s="24" t="s">
         <v>79</v>
@@ -8486,7 +8475,7 @@
       <c r="J57" s="52"/>
     </row>
     <row r="58" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A58" s="61"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="8">
         <v>11</v>
       </c>
@@ -8503,7 +8492,7 @@
       <c r="J58" s="52"/>
     </row>
     <row r="59" spans="1:10" ht="17" customHeight="1">
-      <c r="A59" s="62" t="s">
+      <c r="A59" s="61" t="s">
         <v>92</v>
       </c>
       <c r="B59" s="3">
@@ -8522,12 +8511,12 @@
       <c r="J59" s="52"/>
     </row>
     <row r="60" spans="1:10" ht="16" customHeight="1">
-      <c r="A60" s="63"/>
+      <c r="A60" s="62"/>
       <c r="B60" s="7">
         <v>2</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>23</v>
@@ -8541,7 +8530,7 @@
       <c r="J60" s="52"/>
     </row>
     <row r="61" spans="1:10" ht="16" customHeight="1">
-      <c r="A61" s="63"/>
+      <c r="A61" s="62"/>
       <c r="B61" s="7">
         <v>3</v>
       </c>
@@ -8560,7 +8549,7 @@
       <c r="J61" s="52"/>
     </row>
     <row r="62" spans="1:10" ht="16" customHeight="1">
-      <c r="A62" s="63"/>
+      <c r="A62" s="62"/>
       <c r="B62" s="7">
         <v>4</v>
       </c>
@@ -8577,7 +8566,7 @@
       <c r="J62" s="52"/>
     </row>
     <row r="63" spans="1:10" ht="16" customHeight="1">
-      <c r="A63" s="63"/>
+      <c r="A63" s="62"/>
       <c r="B63" s="7">
         <v>5</v>
       </c>
@@ -8594,7 +8583,7 @@
       <c r="J63" s="52"/>
     </row>
     <row r="64" spans="1:10" ht="16" customHeight="1">
-      <c r="A64" s="63"/>
+      <c r="A64" s="62"/>
       <c r="B64" s="7">
         <v>6</v>
       </c>
@@ -8611,7 +8600,7 @@
       <c r="J64" s="52"/>
     </row>
     <row r="65" spans="1:10" ht="16" customHeight="1">
-      <c r="A65" s="63"/>
+      <c r="A65" s="62"/>
       <c r="B65" s="7">
         <v>7</v>
       </c>
@@ -8630,7 +8619,7 @@
       <c r="J65" s="52"/>
     </row>
     <row r="66" spans="1:10" ht="16" customHeight="1">
-      <c r="A66" s="63"/>
+      <c r="A66" s="62"/>
       <c r="B66" s="7">
         <v>8</v>
       </c>
@@ -8647,7 +8636,7 @@
       <c r="J66" s="52"/>
     </row>
     <row r="67" spans="1:10" ht="16" customHeight="1">
-      <c r="A67" s="63"/>
+      <c r="A67" s="62"/>
       <c r="B67" s="7">
         <v>9</v>
       </c>
@@ -8664,7 +8653,7 @@
       <c r="J67" s="52"/>
     </row>
     <row r="68" spans="1:10" ht="16" customHeight="1">
-      <c r="A68" s="63"/>
+      <c r="A68" s="62"/>
       <c r="B68" s="7">
         <v>10</v>
       </c>
@@ -8681,7 +8670,7 @@
       <c r="J68" s="52"/>
     </row>
     <row r="69" spans="1:10" ht="17" customHeight="1">
-      <c r="A69" s="63"/>
+      <c r="A69" s="62"/>
       <c r="B69" s="7">
         <v>11</v>
       </c>
@@ -8717,10 +8706,10 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D5:D69">
-    <cfRule type="duplicateValues" dxfId="15" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:G74 G5:G69">
-    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8740,7 +8729,7 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -8755,8 +8744,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="93" t="s">
-        <v>517</v>
+      <c r="A1" s="59" t="s">
+        <v>516</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -8796,7 +8785,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="68" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6">
@@ -8810,11 +8799,11 @@
         <v>113</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1">
-      <c r="A6" s="65"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -8830,7 +8819,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1">
-      <c r="A7" s="65"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -8846,7 +8835,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1">
-      <c r="A8" s="65"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -8862,7 +8851,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1">
-      <c r="A9" s="65"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -8880,7 +8869,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1">
-      <c r="A10" s="65"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -8896,7 +8885,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1">
-      <c r="A11" s="65"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -8912,7 +8901,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1">
-      <c r="A12" s="65"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -8926,11 +8915,11 @@
         <v>158</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>339</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1">
-      <c r="A13" s="65"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -8946,7 +8935,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" thickBot="1">
-      <c r="A14" s="66"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="8">
         <v>10</v>
       </c>
@@ -8962,7 +8951,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" customHeight="1">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="68" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6">
@@ -8980,7 +8969,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1">
-      <c r="A16" s="65"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="7">
         <v>2</v>
       </c>
@@ -8998,7 +8987,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1">
-      <c r="A17" s="65"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="7">
         <v>3</v>
       </c>
@@ -9016,7 +9005,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1">
-      <c r="A18" s="65"/>
+      <c r="A18" s="69"/>
       <c r="B18" s="7">
         <v>4</v>
       </c>
@@ -9034,7 +9023,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1">
-      <c r="A19" s="65"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="7">
         <v>5</v>
       </c>
@@ -9046,11 +9035,11 @@
         <v>123</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1">
-      <c r="A20" s="65"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="7">
         <v>6</v>
       </c>
@@ -9058,7 +9047,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>125</v>
@@ -9068,7 +9057,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1">
-      <c r="A21" s="65"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="7">
         <v>7</v>
       </c>
@@ -9080,11 +9069,11 @@
         <v>136</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1">
-      <c r="A22" s="65"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="7">
         <v>8</v>
       </c>
@@ -9100,7 +9089,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1">
-      <c r="A23" s="65"/>
+      <c r="A23" s="69"/>
       <c r="B23" s="7">
         <v>9</v>
       </c>
@@ -9118,7 +9107,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1">
-      <c r="A24" s="65"/>
+      <c r="A24" s="69"/>
       <c r="B24" s="7">
         <v>10</v>
       </c>
@@ -9132,11 +9121,11 @@
         <v>315</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" thickBot="1">
-      <c r="A25" s="66"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="8">
         <v>11</v>
       </c>
@@ -9152,7 +9141,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="68" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="6">
@@ -9172,7 +9161,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1">
-      <c r="A27" s="65"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="7">
         <v>2</v>
       </c>
@@ -9188,7 +9177,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1">
-      <c r="A28" s="65"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="7">
         <v>3</v>
       </c>
@@ -9206,7 +9195,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1">
-      <c r="A29" s="65"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="7">
         <v>4</v>
       </c>
@@ -9222,7 +9211,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1">
-      <c r="A30" s="65"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="7">
         <v>5</v>
       </c>
@@ -9240,7 +9229,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1">
-      <c r="A31" s="65"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="7">
         <v>6</v>
       </c>
@@ -9258,7 +9247,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1">
-      <c r="A32" s="65"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="7">
         <v>7</v>
       </c>
@@ -9274,7 +9263,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" customHeight="1">
-      <c r="A33" s="65"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="7">
         <v>8</v>
       </c>
@@ -9290,7 +9279,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" customHeight="1">
-      <c r="A34" s="65"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="7">
         <v>9</v>
       </c>
@@ -9306,7 +9295,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="16" customHeight="1">
-      <c r="A35" s="65"/>
+      <c r="A35" s="69"/>
       <c r="B35" s="7">
         <v>10</v>
       </c>
@@ -9322,7 +9311,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" customHeight="1" thickBot="1">
-      <c r="A36" s="66"/>
+      <c r="A36" s="70"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -9338,7 +9327,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" customHeight="1">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="68" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="6">
@@ -9356,7 +9345,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" customHeight="1">
-      <c r="A38" s="65"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="7">
         <v>2</v>
       </c>
@@ -9368,11 +9357,11 @@
         <v>200</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" customHeight="1">
-      <c r="A39" s="65"/>
+      <c r="A39" s="69"/>
       <c r="B39" s="7">
         <v>3</v>
       </c>
@@ -9390,7 +9379,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="16" customHeight="1">
-      <c r="A40" s="65"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="7">
         <v>4</v>
       </c>
@@ -9408,7 +9397,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="16" customHeight="1">
-      <c r="A41" s="65"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="7">
         <v>5</v>
       </c>
@@ -9426,7 +9415,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="16" customHeight="1">
-      <c r="A42" s="65"/>
+      <c r="A42" s="69"/>
       <c r="B42" s="7">
         <v>6</v>
       </c>
@@ -9442,7 +9431,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16" customHeight="1">
-      <c r="A43" s="65"/>
+      <c r="A43" s="69"/>
       <c r="B43" s="7">
         <v>7</v>
       </c>
@@ -9458,7 +9447,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="16" customHeight="1">
-      <c r="A44" s="65"/>
+      <c r="A44" s="69"/>
       <c r="B44" s="7">
         <v>8</v>
       </c>
@@ -9474,7 +9463,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" customHeight="1">
-      <c r="A45" s="65"/>
+      <c r="A45" s="69"/>
       <c r="B45" s="7">
         <v>9</v>
       </c>
@@ -9490,7 +9479,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" customHeight="1">
-      <c r="A46" s="65"/>
+      <c r="A46" s="69"/>
       <c r="B46" s="7">
         <v>10</v>
       </c>
@@ -9508,7 +9497,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" customHeight="1" thickBot="1">
-      <c r="A47" s="66"/>
+      <c r="A47" s="70"/>
       <c r="B47" s="8">
         <v>11</v>
       </c>
@@ -9524,7 +9513,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" customHeight="1">
-      <c r="A48" s="64" t="s">
+      <c r="A48" s="68" t="s">
         <v>75</v>
       </c>
       <c r="B48" s="6">
@@ -9538,11 +9527,11 @@
         <v>178</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" customHeight="1">
-      <c r="A49" s="65"/>
+      <c r="A49" s="69"/>
       <c r="B49" s="7">
         <v>2</v>
       </c>
@@ -9560,7 +9549,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" customHeight="1">
-      <c r="A50" s="65"/>
+      <c r="A50" s="69"/>
       <c r="B50" s="7">
         <v>3</v>
       </c>
@@ -9576,7 +9565,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" customHeight="1">
-      <c r="A51" s="65"/>
+      <c r="A51" s="69"/>
       <c r="B51" s="7">
         <v>4</v>
       </c>
@@ -9594,7 +9583,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" customHeight="1">
-      <c r="A52" s="65"/>
+      <c r="A52" s="69"/>
       <c r="B52" s="7">
         <v>5</v>
       </c>
@@ -9610,7 +9599,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" customHeight="1">
-      <c r="A53" s="65"/>
+      <c r="A53" s="69"/>
       <c r="B53" s="7">
         <v>6</v>
       </c>
@@ -9628,7 +9617,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" customHeight="1">
-      <c r="A54" s="65"/>
+      <c r="A54" s="69"/>
       <c r="B54" s="7">
         <v>7</v>
       </c>
@@ -9644,7 +9633,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" customHeight="1">
-      <c r="A55" s="65"/>
+      <c r="A55" s="69"/>
       <c r="B55" s="7">
         <v>8</v>
       </c>
@@ -9660,7 +9649,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="16" customHeight="1">
-      <c r="A56" s="65"/>
+      <c r="A56" s="69"/>
       <c r="B56" s="7">
         <v>9</v>
       </c>
@@ -9678,7 +9667,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" customHeight="1">
-      <c r="A57" s="65"/>
+      <c r="A57" s="69"/>
       <c r="B57" s="7">
         <v>10</v>
       </c>
@@ -9690,11 +9679,11 @@
         <v>162</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16" customHeight="1" thickBot="1">
-      <c r="A58" s="66"/>
+      <c r="A58" s="70"/>
       <c r="B58" s="8">
         <v>11</v>
       </c>
@@ -9710,7 +9699,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" customHeight="1">
-      <c r="A59" s="67" t="s">
+      <c r="A59" s="66" t="s">
         <v>92</v>
       </c>
       <c r="B59" s="3">
@@ -9730,7 +9719,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="16" customHeight="1">
-      <c r="A60" s="68"/>
+      <c r="A60" s="67"/>
       <c r="B60" s="7">
         <v>2</v>
       </c>
@@ -9746,7 +9735,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" customHeight="1">
-      <c r="A61" s="68"/>
+      <c r="A61" s="67"/>
       <c r="B61" s="7">
         <v>3</v>
       </c>
@@ -9764,7 +9753,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" customHeight="1">
-      <c r="A62" s="68"/>
+      <c r="A62" s="67"/>
       <c r="B62" s="7">
         <v>4</v>
       </c>
@@ -9780,7 +9769,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" customHeight="1">
-      <c r="A63" s="68"/>
+      <c r="A63" s="67"/>
       <c r="B63" s="7">
         <v>5</v>
       </c>
@@ -9796,7 +9785,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" customHeight="1">
-      <c r="A64" s="68"/>
+      <c r="A64" s="67"/>
       <c r="B64" s="7">
         <v>6</v>
       </c>
@@ -9814,7 +9803,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" customHeight="1">
-      <c r="A65" s="68"/>
+      <c r="A65" s="67"/>
       <c r="B65" s="7">
         <v>7</v>
       </c>
@@ -9832,7 +9821,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="16" customHeight="1">
-      <c r="A66" s="68"/>
+      <c r="A66" s="67"/>
       <c r="B66" s="7">
         <v>8</v>
       </c>
@@ -9848,7 +9837,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="16" customHeight="1">
-      <c r="A67" s="68"/>
+      <c r="A67" s="67"/>
       <c r="B67" s="7">
         <v>9</v>
       </c>
@@ -9864,7 +9853,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" customHeight="1">
-      <c r="A68" s="68"/>
+      <c r="A68" s="67"/>
       <c r="B68" s="7">
         <v>10</v>
       </c>
@@ -9880,7 +9869,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" customHeight="1">
-      <c r="A69" s="68"/>
+      <c r="A69" s="67"/>
       <c r="B69" s="7">
         <v>11</v>
       </c>
@@ -9888,7 +9877,7 @@
         <v>2</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E69" s="24" t="s">
         <v>144</v>
@@ -9912,7 +9901,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D70:G72 G5:G34 G36:G67 F68:G69">
-    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9932,7 +9921,7 @@
   </sheetPr>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -9949,8 +9938,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="93" t="s">
-        <v>517</v>
+      <c r="A1" s="59" t="s">
+        <v>516</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -9994,10 +9983,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="72">
+      <c r="B5" s="74">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -10013,8 +10002,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="70"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="10" t="s">
         <v>97</v>
       </c>
@@ -10028,8 +10017,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1">
-      <c r="A7" s="70"/>
-      <c r="B7" s="72">
+      <c r="A7" s="77"/>
+      <c r="B7" s="74">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -10045,8 +10034,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
@@ -10060,8 +10049,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="72">
+      <c r="A9" s="77"/>
+      <c r="B9" s="74">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -10077,8 +10066,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A10" s="70"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="10" t="s">
         <v>60</v>
       </c>
@@ -10092,8 +10081,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1">
-      <c r="A11" s="70"/>
-      <c r="B11" s="72">
+      <c r="A11" s="77"/>
+      <c r="B11" s="74">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -10109,8 +10098,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A12" s="70"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
@@ -10124,8 +10113,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1">
-      <c r="A13" s="70"/>
-      <c r="B13" s="72">
+      <c r="A13" s="77"/>
+      <c r="B13" s="74">
         <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -10141,8 +10130,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A14" s="70"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="10" t="s">
         <v>84</v>
       </c>
@@ -10156,8 +10145,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1">
-      <c r="A15" s="70"/>
-      <c r="B15" s="72">
+      <c r="A15" s="77"/>
+      <c r="B15" s="74">
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -10173,8 +10162,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" customHeight="1" thickBot="1">
-      <c r="A16" s="70"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="10" t="s">
         <v>101</v>
       </c>
@@ -10188,8 +10177,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" customHeight="1">
-      <c r="A17" s="70"/>
-      <c r="B17" s="72">
+      <c r="A17" s="77"/>
+      <c r="B17" s="74">
         <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -10205,8 +10194,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A18" s="70"/>
-      <c r="B18" s="73"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="10" t="s">
         <v>245</v>
       </c>
@@ -10220,8 +10209,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" customHeight="1">
-      <c r="A19" s="70"/>
-      <c r="B19" s="72">
+      <c r="A19" s="77"/>
+      <c r="B19" s="74">
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -10237,8 +10226,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A20" s="70"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="10" t="s">
         <v>99</v>
       </c>
@@ -10252,8 +10241,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" customHeight="1">
-      <c r="A21" s="70"/>
-      <c r="B21" s="72">
+      <c r="A21" s="77"/>
+      <c r="B21" s="74">
         <v>9</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -10269,8 +10258,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A22" s="71"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="10" t="s">
         <v>222</v>
       </c>
@@ -10284,10 +10273,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" customHeight="1">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="72">
+      <c r="B23" s="74">
         <v>1</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -10303,8 +10292,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A24" s="70"/>
-      <c r="B24" s="73"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="10" t="s">
         <v>86</v>
       </c>
@@ -10318,8 +10307,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" customHeight="1">
-      <c r="A25" s="70"/>
-      <c r="B25" s="72">
+      <c r="A25" s="77"/>
+      <c r="B25" s="74">
         <v>2</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -10335,8 +10324,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A26" s="70"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="10" t="s">
         <v>58</v>
       </c>
@@ -10350,8 +10339,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" customHeight="1">
-      <c r="A27" s="70"/>
-      <c r="B27" s="72">
+      <c r="A27" s="77"/>
+      <c r="B27" s="74">
         <v>3</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -10367,8 +10356,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A28" s="70"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="10" t="s">
         <v>267</v>
       </c>
@@ -10382,8 +10371,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" customHeight="1">
-      <c r="A29" s="70"/>
-      <c r="B29" s="72">
+      <c r="A29" s="77"/>
+      <c r="B29" s="74">
         <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -10399,8 +10388,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A30" s="70"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="10" t="s">
         <v>64</v>
       </c>
@@ -10414,8 +10403,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" customHeight="1">
-      <c r="A31" s="70"/>
-      <c r="B31" s="72">
+      <c r="A31" s="77"/>
+      <c r="B31" s="74">
         <v>5</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -10431,8 +10420,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A32" s="70"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="10" t="s">
         <v>220</v>
       </c>
@@ -10446,8 +10435,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="16" customHeight="1">
-      <c r="A33" s="70"/>
-      <c r="B33" s="72">
+      <c r="A33" s="77"/>
+      <c r="B33" s="74">
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -10463,8 +10452,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A34" s="70"/>
-      <c r="B34" s="73"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="10" t="s">
         <v>29</v>
       </c>
@@ -10478,8 +10467,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" customHeight="1">
-      <c r="A35" s="70"/>
-      <c r="B35" s="72">
+      <c r="A35" s="77"/>
+      <c r="B35" s="74">
         <v>7</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -10495,8 +10484,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A36" s="70"/>
-      <c r="B36" s="73"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="10" t="s">
         <v>260</v>
       </c>
@@ -10510,8 +10499,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" customHeight="1">
-      <c r="A37" s="70"/>
-      <c r="B37" s="72">
+      <c r="A37" s="77"/>
+      <c r="B37" s="74">
         <v>8</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -10527,8 +10516,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A38" s="70"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="10" t="s">
         <v>253</v>
       </c>
@@ -10542,8 +10531,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" customHeight="1">
-      <c r="A39" s="70"/>
-      <c r="B39" s="72">
+      <c r="A39" s="77"/>
+      <c r="B39" s="74">
         <v>9</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -10559,10 +10548,10 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A40" s="70"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="79"/>
       <c r="C40" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D40" s="10" t="str">
         <f>_xlfn.XLOOKUP(C40,'IND MEN'!$D:$D,'IND MEN'!$E:$E)</f>
@@ -10574,10 +10563,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" customHeight="1">
-      <c r="A41" s="75" t="s">
+      <c r="A41" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="B41" s="72">
+      <c r="B41" s="74">
         <v>1</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -10593,8 +10582,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A42" s="76"/>
-      <c r="B42" s="73"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="10" t="s">
         <v>227</v>
       </c>
@@ -10608,8 +10597,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" customHeight="1">
-      <c r="A43" s="76"/>
-      <c r="B43" s="72">
+      <c r="A43" s="72"/>
+      <c r="B43" s="74">
         <v>2</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -10625,8 +10614,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A44" s="76"/>
-      <c r="B44" s="73"/>
+      <c r="A44" s="72"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="10" t="s">
         <v>16</v>
       </c>
@@ -10640,8 +10629,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" customHeight="1">
-      <c r="A45" s="76"/>
-      <c r="B45" s="72">
+      <c r="A45" s="72"/>
+      <c r="B45" s="74">
         <v>3</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -10657,8 +10646,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A46" s="76"/>
-      <c r="B46" s="73"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="75"/>
       <c r="C46" s="10" t="s">
         <v>247</v>
       </c>
@@ -10672,8 +10661,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" customHeight="1">
-      <c r="A47" s="76"/>
-      <c r="B47" s="72">
+      <c r="A47" s="72"/>
+      <c r="B47" s="74">
         <v>4</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -10689,8 +10678,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A48" s="76"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="75"/>
       <c r="C48" s="10" t="s">
         <v>103</v>
       </c>
@@ -10704,8 +10693,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" customHeight="1">
-      <c r="A49" s="76"/>
-      <c r="B49" s="72">
+      <c r="A49" s="72"/>
+      <c r="B49" s="74">
         <v>5</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -10721,8 +10710,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A50" s="76"/>
-      <c r="B50" s="73"/>
+      <c r="A50" s="72"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="10" t="s">
         <v>78</v>
       </c>
@@ -10736,8 +10725,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="16" customHeight="1">
-      <c r="A51" s="76"/>
-      <c r="B51" s="72">
+      <c r="A51" s="72"/>
+      <c r="B51" s="74">
         <v>6</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -10753,8 +10742,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A52" s="76"/>
-      <c r="B52" s="73"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="10" t="s">
         <v>62</v>
       </c>
@@ -10768,8 +10757,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="16" customHeight="1">
-      <c r="A53" s="76"/>
-      <c r="B53" s="72">
+      <c r="A53" s="72"/>
+      <c r="B53" s="74">
         <v>7</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -10785,8 +10774,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A54" s="76"/>
-      <c r="B54" s="73"/>
+      <c r="A54" s="72"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="10" t="s">
         <v>8</v>
       </c>
@@ -10800,8 +10789,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" customHeight="1">
-      <c r="A55" s="76"/>
-      <c r="B55" s="72">
+      <c r="A55" s="72"/>
+      <c r="B55" s="74">
         <v>8</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -10817,8 +10806,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A56" s="76"/>
-      <c r="B56" s="73"/>
+      <c r="A56" s="72"/>
+      <c r="B56" s="75"/>
       <c r="C56" s="10" t="s">
         <v>236</v>
       </c>
@@ -10832,8 +10821,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" customHeight="1">
-      <c r="A57" s="76"/>
-      <c r="B57" s="72">
+      <c r="A57" s="72"/>
+      <c r="B57" s="74">
         <v>9</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -10849,8 +10838,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="17" customHeight="1" thickBot="1">
-      <c r="A58" s="76"/>
-      <c r="B58" s="73"/>
+      <c r="A58" s="72"/>
+      <c r="B58" s="75"/>
       <c r="C58" s="10" t="s">
         <v>14</v>
       </c>
@@ -10864,8 +10853,8 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="76"/>
-      <c r="B59" s="72">
+      <c r="A59" s="72"/>
+      <c r="B59" s="74">
         <v>10</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -10881,8 +10870,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="17" thickBot="1">
-      <c r="A60" s="77"/>
-      <c r="B60" s="73"/>
+      <c r="A60" s="73"/>
+      <c r="B60" s="75"/>
       <c r="C60" s="10" t="s">
         <v>46</v>
       </c>
@@ -10900,21 +10889,6 @@
     <sortCondition ref="H5:H60"/>
   </sortState>
   <mergeCells count="31">
-    <mergeCell ref="A41:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B21:B22"/>
     <mergeCell ref="A5:A22"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
@@ -10931,10 +10905,25 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A41:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C5:C60">
-    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="22"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.71" right="0.71" top="0.75000000000000011" bottom="0.75000000000000011" header="0.31" footer="0.31"/>
@@ -10957,7 +10946,7 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="142" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="142" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -10973,8 +10962,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23">
-      <c r="A1" s="93" t="s">
-        <v>517</v>
+      <c r="A1" s="59" t="s">
+        <v>516</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -11021,10 +11010,10 @@
       <c r="L4"/>
     </row>
     <row r="5" spans="1:12" ht="16" customHeight="1">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="72">
+      <c r="B5" s="74">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -11044,10 +11033,10 @@
       <c r="L5"/>
     </row>
     <row r="6" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="90"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D6" s="10" t="str">
         <f>_xlfn.XLOOKUP(C6,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11063,8 +11052,8 @@
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" ht="16" customHeight="1">
-      <c r="A7" s="90"/>
-      <c r="B7" s="72">
+      <c r="A7" s="81"/>
+      <c r="B7" s="74">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -11084,8 +11073,8 @@
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A8" s="90"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="10" t="s">
         <v>177</v>
       </c>
@@ -11103,12 +11092,12 @@
       <c r="L8"/>
     </row>
     <row r="9" spans="1:12" ht="16" customHeight="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="72">
+      <c r="A9" s="81"/>
+      <c r="B9" s="74">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D9" s="9" t="str">
         <f>_xlfn.XLOOKUP(C9,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11124,10 +11113,10 @@
       <c r="L9"/>
     </row>
     <row r="10" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A10" s="90"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D10" s="10" t="str">
         <f>_xlfn.XLOOKUP(C10,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11143,8 +11132,8 @@
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" ht="16" customHeight="1">
-      <c r="A11" s="90"/>
-      <c r="B11" s="72">
+      <c r="A11" s="81"/>
+      <c r="B11" s="74">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -11164,8 +11153,8 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A12" s="90"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="10" t="s">
         <v>135</v>
       </c>
@@ -11183,8 +11172,8 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="1:12" ht="16" customHeight="1">
-      <c r="A13" s="90"/>
-      <c r="B13" s="72">
+      <c r="A13" s="81"/>
+      <c r="B13" s="74">
         <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -11204,8 +11193,8 @@
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A14" s="90"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="10" t="s">
         <v>329</v>
       </c>
@@ -11223,8 +11212,8 @@
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" ht="16" customHeight="1">
-      <c r="A15" s="90"/>
-      <c r="B15" s="72">
+      <c r="A15" s="81"/>
+      <c r="B15" s="74">
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -11244,8 +11233,8 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A16" s="90"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="10" t="s">
         <v>143</v>
       </c>
@@ -11263,8 +11252,8 @@
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" ht="16" customHeight="1">
-      <c r="A17" s="90"/>
-      <c r="B17" s="72">
+      <c r="A17" s="81"/>
+      <c r="B17" s="74">
         <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -11284,8 +11273,8 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A18" s="90"/>
-      <c r="B18" s="73"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="10" t="s">
         <v>118</v>
       </c>
@@ -11303,8 +11292,8 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1">
-      <c r="A19" s="90"/>
-      <c r="B19" s="72">
+      <c r="A19" s="81"/>
+      <c r="B19" s="74">
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -11324,8 +11313,8 @@
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A20" s="91"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="10" t="s">
         <v>296</v>
       </c>
@@ -11343,10 +11332,10 @@
       <c r="L20"/>
     </row>
     <row r="21" spans="1:12" ht="16" customHeight="1">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="80" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="72">
+      <c r="B21" s="74">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -11366,10 +11355,10 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A22" s="90"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D22" s="10" t="str">
         <f>_xlfn.XLOOKUP(C22,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11385,8 +11374,8 @@
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="16" customHeight="1">
-      <c r="A23" s="90"/>
-      <c r="B23" s="72">
+      <c r="A23" s="81"/>
+      <c r="B23" s="74">
         <v>2</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -11406,10 +11395,10 @@
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A24" s="90"/>
-      <c r="B24" s="73"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D24" s="10" t="str">
         <f>_xlfn.XLOOKUP(C24,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11425,12 +11414,12 @@
       <c r="L24"/>
     </row>
     <row r="25" spans="1:12" ht="16" customHeight="1">
-      <c r="A25" s="90"/>
-      <c r="B25" s="72">
+      <c r="A25" s="81"/>
+      <c r="B25" s="74">
         <v>3</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D25" s="9" t="str">
         <f>_xlfn.XLOOKUP(C25,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11446,10 +11435,10 @@
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A26" s="90"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D26" s="10" t="str">
         <f>_xlfn.XLOOKUP(C26,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11465,8 +11454,8 @@
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" ht="16" customHeight="1">
-      <c r="A27" s="90"/>
-      <c r="B27" s="72">
+      <c r="A27" s="81"/>
+      <c r="B27" s="74">
         <v>4</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -11486,8 +11475,8 @@
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A28" s="90"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="10" t="s">
         <v>195</v>
       </c>
@@ -11505,12 +11494,12 @@
       <c r="L28"/>
     </row>
     <row r="29" spans="1:12" ht="16" customHeight="1">
-      <c r="A29" s="90"/>
-      <c r="B29" s="72">
+      <c r="A29" s="81"/>
+      <c r="B29" s="74">
         <v>5</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D29" s="9" t="str">
         <f>_xlfn.XLOOKUP(C29,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11526,8 +11515,8 @@
       <c r="L29"/>
     </row>
     <row r="30" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A30" s="90"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="10" t="s">
         <v>114</v>
       </c>
@@ -11545,8 +11534,8 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12" ht="16" customHeight="1">
-      <c r="A31" s="90"/>
-      <c r="B31" s="72">
+      <c r="A31" s="81"/>
+      <c r="B31" s="74">
         <v>6</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -11566,8 +11555,8 @@
       <c r="L31"/>
     </row>
     <row r="32" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A32" s="90"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="10" t="s">
         <v>155</v>
       </c>
@@ -11585,8 +11574,8 @@
       <c r="L32"/>
     </row>
     <row r="33" spans="1:13" ht="16" customHeight="1">
-      <c r="A33" s="90"/>
-      <c r="B33" s="72">
+      <c r="A33" s="81"/>
+      <c r="B33" s="74">
         <v>7</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -11606,8 +11595,8 @@
       <c r="L33"/>
     </row>
     <row r="34" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A34" s="90"/>
-      <c r="B34" s="73"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="10" t="s">
         <v>317</v>
       </c>
@@ -11625,12 +11614,12 @@
       <c r="L34"/>
     </row>
     <row r="35" spans="1:13" ht="16" customHeight="1">
-      <c r="A35" s="90"/>
-      <c r="B35" s="72">
+      <c r="A35" s="81"/>
+      <c r="B35" s="74">
         <v>8</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D35" s="9" t="str">
         <f>_xlfn.XLOOKUP(C35,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11646,8 +11635,8 @@
       <c r="L35"/>
     </row>
     <row r="36" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A36" s="91"/>
-      <c r="B36" s="73"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="10" t="s">
         <v>306</v>
       </c>
@@ -11665,10 +11654,10 @@
       <c r="L36"/>
     </row>
     <row r="37" spans="1:13" ht="16" customHeight="1">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="63" t="s">
         <v>204</v>
       </c>
-      <c r="B37" s="72">
+      <c r="B37" s="74">
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -11688,10 +11677,10 @@
       <c r="L37"/>
     </row>
     <row r="38" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A38" s="60"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D38" s="10" t="str">
         <f>_xlfn.XLOOKUP(C38,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11707,19 +11696,19 @@
       <c r="L38"/>
     </row>
     <row r="39" spans="1:13" ht="16" customHeight="1">
-      <c r="A39" s="60"/>
-      <c r="B39" s="72">
+      <c r="A39" s="64"/>
+      <c r="B39" s="74">
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D39" s="9" t="str">
         <f>_xlfn.XLOOKUP(C39,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
         <v>ミナミ カンナ</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I39" s="11"/>
       <c r="J39"/>
@@ -11727,10 +11716,10 @@
       <c r="L39"/>
     </row>
     <row r="40" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A40" s="60"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="64"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D40" s="10" t="str">
         <f>_xlfn.XLOOKUP(C40,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11746,12 +11735,12 @@
       <c r="L40"/>
     </row>
     <row r="41" spans="1:13" ht="16" customHeight="1">
-      <c r="A41" s="60"/>
-      <c r="B41" s="72">
+      <c r="A41" s="64"/>
+      <c r="B41" s="74">
         <v>3</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D41" s="9" t="str">
         <f>_xlfn.XLOOKUP(C41,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11766,14 +11755,14 @@
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A42" s="60"/>
-      <c r="B42" s="73"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D42" s="10" t="str">
         <f>_xlfn.XLOOKUP(C42,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11789,8 +11778,8 @@
       <c r="L42"/>
     </row>
     <row r="43" spans="1:13" ht="16" customHeight="1">
-      <c r="A43" s="60"/>
-      <c r="B43" s="72">
+      <c r="A43" s="64"/>
+      <c r="B43" s="74">
         <v>4</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -11810,8 +11799,8 @@
       <c r="L43"/>
     </row>
     <row r="44" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A44" s="60"/>
-      <c r="B44" s="73"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="10" t="s">
         <v>173</v>
       </c>
@@ -11829,12 +11818,12 @@
       <c r="L44"/>
     </row>
     <row r="45" spans="1:13" ht="16" customHeight="1">
-      <c r="A45" s="60"/>
-      <c r="B45" s="72">
+      <c r="A45" s="64"/>
+      <c r="B45" s="74">
         <v>5</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D45" s="9" t="str">
         <f>_xlfn.XLOOKUP(C45,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11850,8 +11839,8 @@
       <c r="L45"/>
     </row>
     <row r="46" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A46" s="60"/>
-      <c r="B46" s="73"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="75"/>
       <c r="C46" s="10" t="s">
         <v>333</v>
       </c>
@@ -11869,8 +11858,8 @@
       <c r="L46"/>
     </row>
     <row r="47" spans="1:13" ht="16" customHeight="1">
-      <c r="A47" s="60"/>
-      <c r="B47" s="72">
+      <c r="A47" s="64"/>
+      <c r="B47" s="74">
         <v>6</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -11890,10 +11879,10 @@
       <c r="L47"/>
     </row>
     <row r="48" spans="1:13" ht="17" customHeight="1" thickBot="1">
-      <c r="A48" s="60"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="64"/>
+      <c r="B48" s="75"/>
       <c r="C48" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D48" s="10" t="str">
         <f>_xlfn.XLOOKUP(C48,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11909,12 +11898,12 @@
       <c r="L48"/>
     </row>
     <row r="49" spans="1:12" ht="16" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="72">
+      <c r="A49" s="64"/>
+      <c r="B49" s="74">
         <v>7</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D49" s="9" t="str">
         <f>_xlfn.XLOOKUP(C49,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11930,10 +11919,10 @@
       <c r="L49"/>
     </row>
     <row r="50" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="73"/>
+      <c r="A50" s="64"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D50" s="10" t="str">
         <f>_xlfn.XLOOKUP(C50,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11949,12 +11938,12 @@
       <c r="L50"/>
     </row>
     <row r="51" spans="1:12" ht="16" customHeight="1">
-      <c r="A51" s="60"/>
-      <c r="B51" s="72">
+      <c r="A51" s="64"/>
+      <c r="B51" s="74">
         <v>8</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D51" s="9" t="str">
         <f>_xlfn.XLOOKUP(C51,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -11970,8 +11959,8 @@
       <c r="L51"/>
     </row>
     <row r="52" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A52" s="60"/>
-      <c r="B52" s="73"/>
+      <c r="A52" s="64"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="10" t="s">
         <v>319</v>
       </c>
@@ -11989,8 +11978,8 @@
       <c r="L52"/>
     </row>
     <row r="53" spans="1:12" ht="16" customHeight="1">
-      <c r="A53" s="60"/>
-      <c r="B53" s="72">
+      <c r="A53" s="64"/>
+      <c r="B53" s="74">
         <v>9</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -12006,10 +11995,10 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="17" customHeight="1" thickBot="1">
-      <c r="A54" s="61"/>
-      <c r="B54" s="73"/>
+      <c r="A54" s="65"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D54" s="10" t="str">
         <f>_xlfn.XLOOKUP(C54,'IND WOMEN'!$D:$D,'IND WOMEN'!$E:$E)</f>
@@ -12025,21 +12014,6 @@
     <sortCondition ref="H5:H54"/>
   </sortState>
   <mergeCells count="28">
-    <mergeCell ref="A37:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A5:A20"/>
@@ -12053,12 +12027,25 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A37:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C5:C54">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C54">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
     <cfRule type="duplicateValues" dxfId="9" priority="40"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -12078,7 +12065,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -12092,7 +12079,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -12102,10 +12089,10 @@
     </row>
     <row r="2" spans="1:6" ht="22" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>514</v>
-      </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
+        <v>513</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:6" ht="22" customHeight="1" thickBot="1">
       <c r="C3" s="2"/>
@@ -12122,10 +12109,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="81" t="str">
+      <c r="B5" s="83" t="str">
         <f>_xlfn.XLOOKUP(A5,'IND MEN'!$C:$C,'IND MEN'!$F:$F)</f>
         <v>日本体育大学トランポリンクラブ</v>
       </c>
@@ -12134,31 +12121,31 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="79"/>
-      <c r="B6" s="82"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="79"/>
-      <c r="B7" s="82"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="29" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" thickBot="1">
-      <c r="A8" s="80"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="30" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="81" t="str">
+      <c r="B9" s="83" t="str">
         <f>_xlfn.XLOOKUP(A9,'IND MEN'!$C:$C,'IND MEN'!$F:$F)</f>
         <v>星稜クラブ</v>
       </c>
@@ -12167,31 +12154,31 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20">
-      <c r="A10" s="79"/>
-      <c r="B10" s="82"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="29" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20">
-      <c r="A11" s="79"/>
-      <c r="B11" s="82"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="29" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21" thickBot="1">
-      <c r="A12" s="80"/>
-      <c r="B12" s="83"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="30" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20">
-      <c r="A13" s="78" t="s">
-        <v>518</v>
-      </c>
-      <c r="B13" s="81" t="s">
+      <c r="A13" s="86" t="s">
+        <v>517</v>
+      </c>
+      <c r="B13" s="83" t="s">
         <v>208</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -12199,125 +12186,125 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20">
-      <c r="A14" s="79"/>
-      <c r="B14" s="82"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="29" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20">
-      <c r="A15" s="79"/>
-      <c r="B15" s="82"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" thickBot="1">
-      <c r="A16" s="80"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="C16" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="81" t="s">
-        <v>360</v>
+      <c r="B17" s="83" t="s">
+        <v>359</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20">
-      <c r="A18" s="79"/>
-      <c r="B18" s="82"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20">
-      <c r="A19" s="79"/>
-      <c r="B19" s="82"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" thickBot="1">
-      <c r="A20" s="80"/>
-      <c r="B20" s="83"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="85"/>
       <c r="C20" s="30" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="81" t="s">
-        <v>361</v>
+      <c r="B21" s="83" t="s">
+        <v>360</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20">
-      <c r="A22" s="79"/>
-      <c r="B22" s="82"/>
+      <c r="A22" s="87"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="29" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20">
-      <c r="A23" s="79"/>
-      <c r="B23" s="82"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="29" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" thickBot="1">
-      <c r="A24" s="80"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" ht="20">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="81" t="s">
-        <v>362</v>
+      <c r="B25" s="83" t="s">
+        <v>361</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20">
-      <c r="A26" s="79"/>
-      <c r="B26" s="82"/>
+      <c r="A26" s="87"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="29" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20">
-      <c r="A27" s="79"/>
-      <c r="B27" s="82"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="84"/>
       <c r="C27" s="29" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21" thickBot="1">
-      <c r="A28" s="80"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="83" t="s">
         <v>210</v>
       </c>
       <c r="C29" s="28" t="s">
@@ -12325,26 +12312,32 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="20">
-      <c r="A30" s="79"/>
-      <c r="B30" s="82"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="84"/>
       <c r="C30" s="29" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="20">
-      <c r="A31" s="79"/>
-      <c r="B31" s="82"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="84"/>
       <c r="C31" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21" thickBot="1">
-      <c r="A32" s="80"/>
-      <c r="B32" s="83"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A17:A20"/>
@@ -12353,12 +12346,6 @@
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C5:C11">
@@ -12384,7 +12371,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -12399,7 +12386,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -12409,10 +12396,10 @@
     </row>
     <row r="2" spans="1:6" ht="22" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>515</v>
-      </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
+        <v>514</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:6" ht="22" customHeight="1" thickBot="1">
       <c r="C3" s="2"/>
@@ -12429,10 +12416,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="83" t="s">
         <v>218</v>
       </c>
       <c r="C5" s="28" t="s">
@@ -12440,61 +12427,61 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="79"/>
-      <c r="B6" s="82"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="29" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="79"/>
-      <c r="B7" s="82"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="29" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" thickBot="1">
-      <c r="A8" s="80"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="20">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="81" t="s">
-        <v>364</v>
+      <c r="B9" s="83" t="s">
+        <v>363</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20">
-      <c r="A10" s="79"/>
-      <c r="B10" s="82"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="29" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20">
-      <c r="A11" s="79"/>
-      <c r="B11" s="82"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="29" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21" thickBot="1">
-      <c r="A12" s="80"/>
-      <c r="B12" s="83"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="30" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="86" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="83" t="s">
         <v>208</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -12502,32 +12489,32 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20">
-      <c r="A14" s="79"/>
-      <c r="B14" s="82"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="29" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20">
-      <c r="A15" s="79"/>
-      <c r="B15" s="82"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="29" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" thickBot="1">
-      <c r="A16" s="80"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="C16" s="30" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="81" t="s">
-        <v>360</v>
+      <c r="B17" s="83" t="s">
+        <v>359</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>155</v>
@@ -12535,31 +12522,31 @@
       <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" ht="20">
-      <c r="A18" s="79"/>
-      <c r="B18" s="88"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="31" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20">
-      <c r="A19" s="79"/>
-      <c r="B19" s="82"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="29" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" thickBot="1">
-      <c r="A20" s="80"/>
-      <c r="B20" s="83"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="85"/>
       <c r="C20" s="30" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="20">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="89" t="s">
         <v>336</v>
       </c>
       <c r="C21" s="28" t="s">
@@ -12567,29 +12554,29 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="20">
-      <c r="A22" s="79"/>
-      <c r="B22" s="85"/>
+      <c r="A22" s="87"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="31" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="20">
-      <c r="A23" s="79"/>
-      <c r="B23" s="86"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="29" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" thickBot="1">
-      <c r="A24" s="80"/>
-      <c r="B24" s="87"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="92"/>
       <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:5" ht="20">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="83" t="s">
         <v>216</v>
       </c>
       <c r="C25" s="28" t="s">
@@ -12597,58 +12584,64 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="20">
-      <c r="A26" s="79"/>
-      <c r="B26" s="82"/>
+      <c r="A26" s="87"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="29" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="20">
-      <c r="A27" s="79"/>
-      <c r="B27" s="82"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="84"/>
       <c r="C27" s="29" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" thickBot="1">
-      <c r="A28" s="80"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="20">
-      <c r="A29" s="78" t="s">
-        <v>503</v>
-      </c>
-      <c r="B29" s="81" t="s">
+      <c r="A29" s="86" t="s">
+        <v>502</v>
+      </c>
+      <c r="B29" s="83" t="s">
         <v>210</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="20">
-      <c r="A30" s="79"/>
-      <c r="B30" s="82"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="84"/>
       <c r="C30" s="29" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="20">
-      <c r="A31" s="79"/>
-      <c r="B31" s="82"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="84"/>
       <c r="C31" s="29" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="21" thickBot="1">
-      <c r="A32" s="80"/>
-      <c r="B32" s="83"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="30" t="s">
         <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="A21:A24"/>
@@ -12657,12 +12650,6 @@
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C5:C8">
@@ -12708,10 +12695,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19">
       <c r="A1" s="48" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1" s="48" t="s">
         <v>370</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>371</v>
       </c>
       <c r="C1" s="49" t="str">
         <f>_xlfn.CONCAT(A1," ",B1)</f>
@@ -12728,10 +12715,10 @@
     </row>
     <row r="2" spans="1:6" ht="19">
       <c r="A2" s="48" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>373</v>
       </c>
       <c r="C2" s="49" t="str">
         <f t="shared" ref="C2:C65" si="0">_xlfn.CONCAT(A2," ",B2)</f>
@@ -12748,10 +12735,10 @@
     </row>
     <row r="3" spans="1:6" ht="19">
       <c r="A3" s="48" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>374</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>375</v>
       </c>
       <c r="C3" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12768,10 +12755,10 @@
     </row>
     <row r="4" spans="1:6" ht="19">
       <c r="A4" s="48" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>376</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>377</v>
       </c>
       <c r="C4" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12788,10 +12775,10 @@
     </row>
     <row r="5" spans="1:6" ht="19">
       <c r="A5" s="48" t="s">
+        <v>377</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>378</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>379</v>
       </c>
       <c r="C5" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12808,10 +12795,10 @@
     </row>
     <row r="6" spans="1:6" ht="19">
       <c r="A6" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>380</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>381</v>
       </c>
       <c r="C6" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12823,15 +12810,15 @@
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="51" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19">
       <c r="A7" s="48" t="s">
+        <v>382</v>
+      </c>
+      <c r="B7" s="48" t="s">
         <v>383</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>384</v>
       </c>
       <c r="C7" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12848,10 +12835,10 @@
     </row>
     <row r="8" spans="1:6" ht="19">
       <c r="A8" s="48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="48" t="s">
         <v>385</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>386</v>
       </c>
       <c r="C8" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12868,10 +12855,10 @@
     </row>
     <row r="9" spans="1:6" ht="19">
       <c r="A9" s="48" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" s="48" t="s">
         <v>387</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>388</v>
       </c>
       <c r="C9" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12888,10 +12875,10 @@
     </row>
     <row r="10" spans="1:6" ht="19">
       <c r="A10" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>389</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>390</v>
       </c>
       <c r="C10" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12908,10 +12895,10 @@
     </row>
     <row r="11" spans="1:6" ht="19">
       <c r="A11" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>391</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>392</v>
       </c>
       <c r="C11" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12928,10 +12915,10 @@
     </row>
     <row r="12" spans="1:6" ht="19">
       <c r="A12" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" s="48" t="s">
         <v>393</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>394</v>
       </c>
       <c r="C12" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12948,10 +12935,10 @@
     </row>
     <row r="13" spans="1:6" ht="19">
       <c r="A13" s="48" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" s="48" t="s">
         <v>395</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>396</v>
       </c>
       <c r="C13" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12968,10 +12955,10 @@
     </row>
     <row r="14" spans="1:6" ht="19">
       <c r="A14" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>391</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>392</v>
       </c>
       <c r="C14" s="49" t="str">
         <f t="shared" si="0"/>
@@ -12988,10 +12975,10 @@
     </row>
     <row r="15" spans="1:6" ht="19">
       <c r="A15" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="B15" s="48" t="s">
         <v>397</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>398</v>
       </c>
       <c r="C15" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13008,10 +12995,10 @@
     </row>
     <row r="16" spans="1:6" ht="19">
       <c r="A16" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="B16" s="48" t="s">
         <v>399</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>400</v>
       </c>
       <c r="C16" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13028,10 +13015,10 @@
     </row>
     <row r="17" spans="1:6" ht="19">
       <c r="A17" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="B17" s="48" t="s">
         <v>401</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>402</v>
       </c>
       <c r="C17" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13048,10 +13035,10 @@
     </row>
     <row r="18" spans="1:6" ht="19">
       <c r="A18" s="48" t="s">
+        <v>402</v>
+      </c>
+      <c r="B18" s="48" t="s">
         <v>403</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>404</v>
       </c>
       <c r="C18" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13068,10 +13055,10 @@
     </row>
     <row r="19" spans="1:6" ht="19">
       <c r="A19" s="48" t="s">
+        <v>404</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>405</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>406</v>
       </c>
       <c r="C19" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13088,10 +13075,10 @@
     </row>
     <row r="20" spans="1:6" ht="19">
       <c r="A20" s="48" t="s">
+        <v>406</v>
+      </c>
+      <c r="B20" s="48" t="s">
         <v>407</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>408</v>
       </c>
       <c r="C20" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13108,10 +13095,10 @@
     </row>
     <row r="21" spans="1:6" ht="19">
       <c r="A21" s="48" t="s">
+        <v>408</v>
+      </c>
+      <c r="B21" s="48" t="s">
         <v>409</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>410</v>
       </c>
       <c r="C21" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13128,10 +13115,10 @@
     </row>
     <row r="22" spans="1:6" ht="19">
       <c r="A22" s="48" t="s">
+        <v>410</v>
+      </c>
+      <c r="B22" s="48" t="s">
         <v>411</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>412</v>
       </c>
       <c r="C22" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13148,10 +13135,10 @@
     </row>
     <row r="23" spans="1:6" ht="19">
       <c r="A23" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="B23" s="48" t="s">
         <v>413</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>414</v>
       </c>
       <c r="C23" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13168,10 +13155,10 @@
     </row>
     <row r="24" spans="1:6" ht="19">
       <c r="A24" s="48" t="s">
+        <v>414</v>
+      </c>
+      <c r="B24" s="48" t="s">
         <v>415</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>416</v>
       </c>
       <c r="C24" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13188,10 +13175,10 @@
     </row>
     <row r="25" spans="1:6" ht="19">
       <c r="A25" s="48" t="s">
+        <v>416</v>
+      </c>
+      <c r="B25" s="48" t="s">
         <v>417</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>418</v>
       </c>
       <c r="C25" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13208,10 +13195,10 @@
     </row>
     <row r="26" spans="1:6" ht="19">
       <c r="A26" s="48" t="s">
+        <v>418</v>
+      </c>
+      <c r="B26" s="48" t="s">
         <v>419</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>420</v>
       </c>
       <c r="C26" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13223,15 +13210,15 @@
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="51" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="19">
       <c r="A27" s="48" t="s">
+        <v>421</v>
+      </c>
+      <c r="B27" s="48" t="s">
         <v>422</v>
-      </c>
-      <c r="B27" s="48" t="s">
-        <v>423</v>
       </c>
       <c r="C27" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13248,10 +13235,10 @@
     </row>
     <row r="28" spans="1:6" ht="19">
       <c r="A28" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>424</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>425</v>
       </c>
       <c r="C28" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13268,10 +13255,10 @@
     </row>
     <row r="29" spans="1:6" ht="19">
       <c r="A29" s="48" t="s">
+        <v>425</v>
+      </c>
+      <c r="B29" s="48" t="s">
         <v>426</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>427</v>
       </c>
       <c r="C29" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13283,15 +13270,15 @@
       </c>
       <c r="E29" s="50"/>
       <c r="F29" s="51" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="19">
       <c r="A30" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="B30" s="48" t="s">
         <v>429</v>
-      </c>
-      <c r="B30" s="48" t="s">
-        <v>430</v>
       </c>
       <c r="C30" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13308,10 +13295,10 @@
     </row>
     <row r="31" spans="1:6" ht="19">
       <c r="A31" s="48" t="s">
+        <v>430</v>
+      </c>
+      <c r="B31" s="48" t="s">
         <v>431</v>
-      </c>
-      <c r="B31" s="48" t="s">
-        <v>432</v>
       </c>
       <c r="C31" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13328,10 +13315,10 @@
     </row>
     <row r="32" spans="1:6" ht="19">
       <c r="A32" s="48" t="s">
+        <v>432</v>
+      </c>
+      <c r="B32" s="48" t="s">
         <v>433</v>
-      </c>
-      <c r="B32" s="48" t="s">
-        <v>434</v>
       </c>
       <c r="C32" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13348,10 +13335,10 @@
     </row>
     <row r="33" spans="1:6" ht="19">
       <c r="A33" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="B33" s="48" t="s">
         <v>435</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>436</v>
       </c>
       <c r="C33" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13368,10 +13355,10 @@
     </row>
     <row r="34" spans="1:6" ht="19">
       <c r="A34" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="B34" s="48" t="s">
         <v>437</v>
-      </c>
-      <c r="B34" s="48" t="s">
-        <v>438</v>
       </c>
       <c r="C34" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13388,10 +13375,10 @@
     </row>
     <row r="35" spans="1:6" ht="19">
       <c r="A35" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="B35" s="48" t="s">
         <v>439</v>
-      </c>
-      <c r="B35" s="48" t="s">
-        <v>440</v>
       </c>
       <c r="C35" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13408,10 +13395,10 @@
     </row>
     <row r="36" spans="1:6" ht="19">
       <c r="A36" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="B36" s="48" t="s">
         <v>441</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>442</v>
       </c>
       <c r="C36" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13428,10 +13415,10 @@
     </row>
     <row r="37" spans="1:6" ht="19">
       <c r="A37" s="48" t="s">
+        <v>442</v>
+      </c>
+      <c r="B37" s="48" t="s">
         <v>443</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>444</v>
       </c>
       <c r="C37" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13448,10 +13435,10 @@
     </row>
     <row r="38" spans="1:6" ht="19">
       <c r="A38" s="48" t="s">
+        <v>444</v>
+      </c>
+      <c r="B38" s="48" t="s">
         <v>445</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>446</v>
       </c>
       <c r="C38" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13463,15 +13450,15 @@
       </c>
       <c r="E38" s="50"/>
       <c r="F38" s="51" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="19">
       <c r="A39" s="48" t="s">
+        <v>447</v>
+      </c>
+      <c r="B39" s="48" t="s">
         <v>448</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>449</v>
       </c>
       <c r="C39" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13488,10 +13475,10 @@
     </row>
     <row r="40" spans="1:6" ht="19">
       <c r="A40" s="48" t="s">
+        <v>449</v>
+      </c>
+      <c r="B40" s="48" t="s">
         <v>450</v>
-      </c>
-      <c r="B40" s="48" t="s">
-        <v>451</v>
       </c>
       <c r="C40" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13508,10 +13495,10 @@
     </row>
     <row r="41" spans="1:6" ht="19">
       <c r="A41" s="48" t="s">
+        <v>451</v>
+      </c>
+      <c r="B41" s="48" t="s">
         <v>452</v>
-      </c>
-      <c r="B41" s="48" t="s">
-        <v>453</v>
       </c>
       <c r="C41" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13528,10 +13515,10 @@
     </row>
     <row r="42" spans="1:6" ht="19">
       <c r="A42" s="48" t="s">
+        <v>453</v>
+      </c>
+      <c r="B42" s="48" t="s">
         <v>454</v>
-      </c>
-      <c r="B42" s="48" t="s">
-        <v>455</v>
       </c>
       <c r="C42" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13548,10 +13535,10 @@
     </row>
     <row r="43" spans="1:6" ht="19">
       <c r="A43" s="48" t="s">
+        <v>455</v>
+      </c>
+      <c r="B43" s="48" t="s">
         <v>456</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>457</v>
       </c>
       <c r="C43" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13563,15 +13550,15 @@
       </c>
       <c r="E43" s="50"/>
       <c r="F43" s="51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="19">
       <c r="A44" s="48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C44" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13588,10 +13575,10 @@
     </row>
     <row r="45" spans="1:6" ht="19">
       <c r="A45" s="48" t="s">
+        <v>459</v>
+      </c>
+      <c r="B45" s="48" t="s">
         <v>460</v>
-      </c>
-      <c r="B45" s="48" t="s">
-        <v>461</v>
       </c>
       <c r="C45" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13603,15 +13590,15 @@
       </c>
       <c r="E45" s="50"/>
       <c r="F45" s="51" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="19">
       <c r="A46" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="B46" s="48" t="s">
         <v>463</v>
-      </c>
-      <c r="B46" s="48" t="s">
-        <v>464</v>
       </c>
       <c r="C46" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13628,10 +13615,10 @@
     </row>
     <row r="47" spans="1:6" ht="19">
       <c r="A47" s="48" t="s">
+        <v>464</v>
+      </c>
+      <c r="B47" s="48" t="s">
         <v>465</v>
-      </c>
-      <c r="B47" s="48" t="s">
-        <v>466</v>
       </c>
       <c r="C47" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13648,10 +13635,10 @@
     </row>
     <row r="48" spans="1:6" ht="19">
       <c r="A48" s="48" t="s">
+        <v>466</v>
+      </c>
+      <c r="B48" s="48" t="s">
         <v>467</v>
-      </c>
-      <c r="B48" s="48" t="s">
-        <v>468</v>
       </c>
       <c r="C48" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13668,10 +13655,10 @@
     </row>
     <row r="49" spans="1:6" ht="19">
       <c r="A49" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="B49" s="48" t="s">
         <v>469</v>
-      </c>
-      <c r="B49" s="48" t="s">
-        <v>470</v>
       </c>
       <c r="C49" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13688,10 +13675,10 @@
     </row>
     <row r="50" spans="1:6" ht="19">
       <c r="A50" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="B50" s="48" t="s">
         <v>471</v>
-      </c>
-      <c r="B50" s="48" t="s">
-        <v>472</v>
       </c>
       <c r="C50" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13708,10 +13695,10 @@
     </row>
     <row r="51" spans="1:6" ht="19">
       <c r="A51" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C51" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13723,15 +13710,15 @@
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="51" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="19">
       <c r="A52" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="B52" s="48" t="s">
         <v>474</v>
-      </c>
-      <c r="B52" s="48" t="s">
-        <v>475</v>
       </c>
       <c r="C52" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13748,10 +13735,10 @@
     </row>
     <row r="53" spans="1:6" ht="19">
       <c r="A53" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="B53" s="48" t="s">
         <v>476</v>
-      </c>
-      <c r="B53" s="48" t="s">
-        <v>477</v>
       </c>
       <c r="C53" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13768,10 +13755,10 @@
     </row>
     <row r="54" spans="1:6" ht="19">
       <c r="A54" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C54" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13788,10 +13775,10 @@
     </row>
     <row r="55" spans="1:6" ht="19">
       <c r="A55" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="B55" s="48" t="s">
         <v>479</v>
-      </c>
-      <c r="B55" s="48" t="s">
-        <v>480</v>
       </c>
       <c r="C55" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13808,10 +13795,10 @@
     </row>
     <row r="56" spans="1:6" ht="19">
       <c r="A56" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="B56" s="48" t="s">
         <v>481</v>
-      </c>
-      <c r="B56" s="48" t="s">
-        <v>482</v>
       </c>
       <c r="C56" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13828,10 +13815,10 @@
     </row>
     <row r="57" spans="1:6" ht="19">
       <c r="A57" s="48" t="s">
+        <v>482</v>
+      </c>
+      <c r="B57" s="48" t="s">
         <v>483</v>
-      </c>
-      <c r="B57" s="48" t="s">
-        <v>484</v>
       </c>
       <c r="C57" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13848,10 +13835,10 @@
     </row>
     <row r="58" spans="1:6" ht="19">
       <c r="A58" s="48" t="s">
+        <v>484</v>
+      </c>
+      <c r="B58" s="48" t="s">
         <v>485</v>
-      </c>
-      <c r="B58" s="48" t="s">
-        <v>486</v>
       </c>
       <c r="C58" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13868,10 +13855,10 @@
     </row>
     <row r="59" spans="1:6" ht="19">
       <c r="A59" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C59" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13888,10 +13875,10 @@
     </row>
     <row r="60" spans="1:6" ht="19">
       <c r="A60" s="48" t="s">
+        <v>487</v>
+      </c>
+      <c r="B60" s="48" t="s">
         <v>488</v>
-      </c>
-      <c r="B60" s="48" t="s">
-        <v>489</v>
       </c>
       <c r="C60" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13903,15 +13890,15 @@
       </c>
       <c r="E60" s="50"/>
       <c r="F60" s="51" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="19">
       <c r="A61" s="48" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C61" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13928,10 +13915,10 @@
     </row>
     <row r="62" spans="1:6" ht="19">
       <c r="A62" s="48" t="s">
+        <v>491</v>
+      </c>
+      <c r="B62" s="48" t="s">
         <v>492</v>
-      </c>
-      <c r="B62" s="48" t="s">
-        <v>493</v>
       </c>
       <c r="C62" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13948,10 +13935,10 @@
     </row>
     <row r="63" spans="1:6" ht="19">
       <c r="A63" s="48" t="s">
+        <v>493</v>
+      </c>
+      <c r="B63" s="48" t="s">
         <v>494</v>
-      </c>
-      <c r="B63" s="48" t="s">
-        <v>495</v>
       </c>
       <c r="C63" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13968,10 +13955,10 @@
     </row>
     <row r="64" spans="1:6" ht="19">
       <c r="A64" s="48" t="s">
+        <v>495</v>
+      </c>
+      <c r="B64" s="48" t="s">
         <v>496</v>
-      </c>
-      <c r="B64" s="48" t="s">
-        <v>497</v>
       </c>
       <c r="C64" s="49" t="str">
         <f t="shared" si="0"/>
@@ -13988,10 +13975,10 @@
     </row>
     <row r="65" spans="1:6" ht="19">
       <c r="A65" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="B65" s="48" t="s">
         <v>498</v>
-      </c>
-      <c r="B65" s="48" t="s">
-        <v>499</v>
       </c>
       <c r="C65" s="49" t="str">
         <f t="shared" si="0"/>
@@ -14008,10 +13995,10 @@
     </row>
     <row r="66" spans="1:6" ht="19">
       <c r="A66" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="B66" s="48" t="s">
         <v>500</v>
-      </c>
-      <c r="B66" s="48" t="s">
-        <v>501</v>
       </c>
       <c r="C66" s="49" t="str">
         <f t="shared" ref="C66" si="1">_xlfn.CONCAT(A66," ",B66)</f>
@@ -14102,14 +14089,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="952e7e5e-963e-4d92-84b7-491b93135911">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1b7a6422-acb0-42a5-b83e-dbe86ecd454b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14356,27 +14341,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="952e7e5e-963e-4d92-84b7-491b93135911">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1b7a6422-acb0-42a5-b83e-dbe86ecd454b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96297B6E-17FE-4143-BFBF-159E92404910}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82E2AAF0-2B82-434E-941D-DDA77660856D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="952e7e5e-963e-4d92-84b7-491b93135911"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1b7a6422-acb0-42a5-b83e-dbe86ecd454b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14401,9 +14379,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82E2AAF0-2B82-434E-941D-DDA77660856D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96297B6E-17FE-4143-BFBF-159E92404910}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="952e7e5e-963e-4d92-84b7-491b93135911"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1b7a6422-acb0-42a5-b83e-dbe86ecd454b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>